<commit_message>
Updated on 8 Jul
</commit_message>
<xml_diff>
--- a/demos2.xlsx
+++ b/demos2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsui/Documents/GitHub/atsuihk.github.io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\atsuihk.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFC6475-3FC7-F146-B639-CB1A72792493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC958164-2DDF-4897-A369-8B08D7323945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="28240" windowHeight="16080" xr2:uid="{78869667-DC14-C34D-8E40-751570D61855}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{78869667-DC14-C34D-8E40-751570D61855}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Picture</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,34 +54,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Will be available soon…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://endlessicons.com/wp-content/uploads/2012/11/loading-icon-614x460.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Sunshining Analysis for Hong Kong Public Buses (Geoprocessing Toolbox for ArcGIS Pro)</t>
+  </si>
+  <si>
+    <t>A geoprocessing toolbox for finding which side (Left / Right) of bus is under sunlight exposure in Hong Kong.</t>
+  </si>
+  <si>
+    <t>https://github.com/atsuihk/hkbus</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/a1.png</t>
+  </si>
+  <si>
+    <t>Drone location generator for Hong Kong</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/atsuihk/atsuihk.github.io/main/pics/a2.png</t>
+  </si>
+  <si>
+    <t>Python scripts to generate drone location and routes upon Hong Kong's air according to terrain.</t>
+  </si>
+  <si>
+    <t>https://github.com/atsuihk/drones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -96,7 +108,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -142,8 +154,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -159,7 +171,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -477,19 +489,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35B43E3-CBE3-1E4D-8272-02E2CB7B0D41}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="49.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="49.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="52" style="3" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="56.6328125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,38 +515,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17">
+    <row r="2" spans="1:4" ht="31" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
-      <c r="D3" s="2"/>
+    <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{661C4C89-4B2A-3C48-A11B-4298D1F73AE2}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{AAAEADD9-2496-4215-A737-ACC37AFEF4E6}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{B2C84BD6-4850-47D8-A34B-BCE54DEFFFCB}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{E67DE938-EF3A-4CB5-BD2E-53E30BC7112B}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{4AC1D323-37D5-40FF-A7B2-84323D153A5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>